<commit_message>
Rettelser under vejledning med Anders
Co-Authored-By: thundergrove <thundergrove@users.noreply.github.com>
Co-Authored-By: Mik Pedersen <mikpedersen@users.noreply.github.com>
Co-Authored-By: Rasmus Jannerup <rasm211d@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/05 Test/ATD01 Vis Beskedhistorik.xlsx
+++ b/05 Test/ATD01 Vis Beskedhistorik.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emiln\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emiln\Dokumenter\1AarsProjekt\05 Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4196914-A62D-4F89-97EC-E56BAA2816B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D84AC66-E420-455C-AFB1-01486C7820E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{7664EDD4-4E5D-4982-A078-173EE846B630}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7664EDD4-4E5D-4982-A078-173EE846B630}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Tests til UC01</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Antal beskeder = 0</t>
   </si>
   <si>
-    <t>"Ingen beskeder i historikken"</t>
-  </si>
-  <si>
     <t>TC2</t>
   </si>
   <si>
@@ -82,6 +79,96 @@
   </si>
   <si>
     <t>Patientoversigt vises</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t>Ny beskedhistorik for Tom Jensen</t>
+  </si>
+  <si>
+    <t>beskeder.size = 0</t>
+  </si>
+  <si>
+    <t>patient = Tom Jensen</t>
+  </si>
+  <si>
+    <t>TC6</t>
+  </si>
+  <si>
+    <t>beskedhistorik.tilfoejBesked(besked, patient)</t>
+  </si>
+  <si>
+    <t>beskeder.size = 1</t>
+  </si>
+  <si>
+    <t>TC7</t>
+  </si>
+  <si>
+    <t>besked = null</t>
+  </si>
+  <si>
+    <t>BeskedErNullException</t>
+  </si>
+  <si>
+    <t>patient = null</t>
+  </si>
+  <si>
+    <t>PatientErNullException</t>
+  </si>
+  <si>
+    <t>TC8</t>
+  </si>
+  <si>
+    <t>TC9</t>
+  </si>
+  <si>
+    <t>Ny beskedhistorik for null</t>
+  </si>
+  <si>
+    <t>besked.tekst = "tekst"</t>
+  </si>
+  <si>
+    <t>besked:</t>
+  </si>
+  <si>
+    <t>besked.afsender = Tom Jensen</t>
+  </si>
+  <si>
+    <t>besked.datotid = 2020-05-22 15:10</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>besked2:</t>
+  </si>
+  <si>
+    <t>besked2.tekst = "tekst"</t>
+  </si>
+  <si>
+    <t>besked2.afsender = Tom Jensen</t>
+  </si>
+  <si>
+    <t>besked2.datotid = 2020-05-22 14:00</t>
+  </si>
+  <si>
+    <t>beskedhistorik.tilfoejBesked(besked2, patient)</t>
+  </si>
+  <si>
+    <t>beskeder.size = 2</t>
+  </si>
+  <si>
+    <t>beskeder[0].datotid = 2020-05-22 14:00</t>
+  </si>
+  <si>
+    <t>beskeder[1].datotid = 2020-05-22 15:10</t>
+  </si>
+  <si>
+    <t>"Ingen beskeder"</t>
+  </si>
+  <si>
+    <t>beskedhistorik for Tom Jensen</t>
   </si>
 </sst>
 </file>
@@ -123,7 +210,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +220,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -207,14 +300,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,16 +631,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8133992-CCEF-4807-8D12-12D1FB1B8EA1}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.5703125" customWidth="1"/>
     <col min="3" max="3" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -552,73 +650,280 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C6" s="11"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="11"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="5"/>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Del ATD og UTD og i hver sit artefakt
Closes #52
</commit_message>
<xml_diff>
--- a/05 Test/ATD01 Vis Beskedhistorik.xlsx
+++ b/05 Test/ATD01 Vis Beskedhistorik.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emiln\Dokumenter\1AarsProjekt\05 Test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/95ef811b0cfc9726/Skrivebord/1aarsprojekt/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D84AC66-E420-455C-AFB1-01486C7820E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EFDD6E1A-1AD6-440C-9344-A9ACEF5D8BD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7664EDD4-4E5D-4982-A078-173EE846B630}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7664EDD4-4E5D-4982-A078-173EE846B630}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Tests til UC01</t>
   </si>
@@ -81,94 +81,7 @@
     <t>Patientoversigt vises</t>
   </si>
   <si>
-    <t>TC5</t>
-  </si>
-  <si>
-    <t>Ny beskedhistorik for Tom Jensen</t>
-  </si>
-  <si>
-    <t>beskeder.size = 0</t>
-  </si>
-  <si>
-    <t>patient = Tom Jensen</t>
-  </si>
-  <si>
-    <t>TC6</t>
-  </si>
-  <si>
-    <t>beskedhistorik.tilfoejBesked(besked, patient)</t>
-  </si>
-  <si>
-    <t>beskeder.size = 1</t>
-  </si>
-  <si>
-    <t>TC7</t>
-  </si>
-  <si>
-    <t>besked = null</t>
-  </si>
-  <si>
-    <t>BeskedErNullException</t>
-  </si>
-  <si>
-    <t>patient = null</t>
-  </si>
-  <si>
-    <t>PatientErNullException</t>
-  </si>
-  <si>
-    <t>TC8</t>
-  </si>
-  <si>
-    <t>TC9</t>
-  </si>
-  <si>
-    <t>Ny beskedhistorik for null</t>
-  </si>
-  <si>
-    <t>besked.tekst = "tekst"</t>
-  </si>
-  <si>
-    <t>besked:</t>
-  </si>
-  <si>
-    <t>besked.afsender = Tom Jensen</t>
-  </si>
-  <si>
-    <t>besked.datotid = 2020-05-22 15:10</t>
-  </si>
-  <si>
-    <t>TC10</t>
-  </si>
-  <si>
-    <t>besked2:</t>
-  </si>
-  <si>
-    <t>besked2.tekst = "tekst"</t>
-  </si>
-  <si>
-    <t>besked2.afsender = Tom Jensen</t>
-  </si>
-  <si>
-    <t>besked2.datotid = 2020-05-22 14:00</t>
-  </si>
-  <si>
-    <t>beskedhistorik.tilfoejBesked(besked2, patient)</t>
-  </si>
-  <si>
-    <t>beskeder.size = 2</t>
-  </si>
-  <si>
-    <t>beskeder[0].datotid = 2020-05-22 14:00</t>
-  </si>
-  <si>
-    <t>beskeder[1].datotid = 2020-05-22 15:10</t>
-  </si>
-  <si>
     <t>"Ingen beskeder"</t>
-  </si>
-  <si>
-    <t>beskedhistorik for Tom Jensen</t>
   </si>
 </sst>
 </file>
@@ -300,14 +213,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -631,25 +541,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8133992-CCEF-4807-8D12-12D1FB1B8EA1}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="51.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="51.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -660,270 +570,235 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="11"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="11"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>